<commit_message>
Start without being random
</commit_message>
<xml_diff>
--- a/data/teacher/Andre Barros.xlsx
+++ b/data/teacher/Andre Barros.xlsx
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EAP - MCT-2A</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -606,22 +606,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>EAP - MEC-3A</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAP - MCT-2A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Start of pontuation system
</commit_message>
<xml_diff>
--- a/data/teacher/Andre Barros.xlsx
+++ b/data/teacher/Andre Barros.xlsx
@@ -520,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAP - MEC-3A</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAP - MEC-3A</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>EAP - MEC-3A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">

</xml_diff>

<commit_message>
Fix of the two same subjects
</commit_message>
<xml_diff>
--- a/data/teacher/Andre Barros.xlsx
+++ b/data/teacher/Andre Barros.xlsx
@@ -520,12 +520,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>MCT-2A-EAP</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>MEC-3A-EAP</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -552,12 +552,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>MCT-2A-EAP</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>MEC-3A-EAP</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
6 hours by turn fix
</commit_message>
<xml_diff>
--- a/data/teacher/Andre Barros.xlsx
+++ b/data/teacher/Andre Barros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,27 +505,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>MEC-3A-EAP</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>MCT-2A-EAP</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>MCT-2A-EAP</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>MEC-3A-EAP</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MEC-3A-EAP</t>
+          <t>MCT-2A-EAP</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MEC-3A-EAP</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -665,66 +665,66 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Almoço</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Almoço</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Almoço</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Almoço</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Almoço</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Almoço</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Almoço</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Almoço</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Almoço</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Almoço</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -756,7 +756,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -788,98 +788,174 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>14:40</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Intervalo</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Intervalo</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Intervalo</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Intervalo</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Intervalo</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>15:50</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Intervalo</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Intervalo</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Intervalo</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Intervalo</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Intervalo</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>15:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>16:40</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>18:20</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Full logic part of bimestral classes
</commit_message>
<xml_diff>
--- a/data/teacher/Andre Barros.xlsx
+++ b/data/teacher/Andre Barros.xlsx
@@ -510,22 +510,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>MCT-2A-EAP</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>MEC-3A-EAP</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MCT-2A-EAP</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MEC-3A-EAP</t>
+          <t>MCT-2A-EAP</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MEC-3A-EAP</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MEC-3A-EAP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">

</xml_diff>